<commit_message>
Latest data: for Scottish Tue May 25 17:42:39 UTC 2021
</commit_message>
<xml_diff>
--- a/uk/scotland/COVID-19%2Bdaily%2Bdata%2B-%2Bby%2BNHS%2BBoard%2B-%2B25%2BMay%2B2021.xlsx
+++ b/uk/scotland/COVID-19%2Bdaily%2Bdata%2B-%2Bby%2BNHS%2BBoard%2B-%2B25%2BMay%2B2021.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10042" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10044" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>Please see note C25 on the notes page.</t>
+  </si>
+  <si>
+    <t>Please see note H36 on notes page regarding correction of NHS Borders figure.</t>
   </si>
 </sst>
 </file>
@@ -1043,15 +1046,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>654050</xdr:colOff>
+      <xdr:colOff>625475</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>156210</xdr:colOff>
-      <xdr:row>221</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1060,8 +1063,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="654050" y="231774"/>
-          <a:ext cx="7426960" cy="40535226"/>
+          <a:off x="625475" y="238124"/>
+          <a:ext cx="7074535" cy="42929176"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4972,7 +4975,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>H35. </a:t>
+            <a:t>H.35 </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" i="0">
@@ -5001,9 +5004,42 @@
             </a:rPr>
             <a:t>. </a:t>
           </a:r>
-          <a:endParaRPr lang="en-GB">
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" i="0">
             <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>H.36 The figure for NHS Borders was initially published erroneously as 9 (on 25/05/2021). This has been revised to * which denotes less than 5, in line with the disclosure control policy for covid reporting.</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -45715,7 +45751,7 @@
   <dimension ref="A1:S260"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="C232" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B235" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" sqref="A1:I1"/>
@@ -59284,7 +59320,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A257" s="36">
         <v>44338</v>
       </c>
@@ -59337,7 +59373,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="258" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A258" s="36">
         <v>44339</v>
       </c>
@@ -59390,7 +59426,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="259" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A259" s="36">
         <v>44340</v>
       </c>
@@ -59443,15 +59479,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="260" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A260" s="36">
         <v>44341</v>
       </c>
       <c r="B260" s="99">
         <v>9</v>
       </c>
-      <c r="C260" s="99">
-        <v>9</v>
+      <c r="C260" s="99" t="s">
+        <v>25</v>
       </c>
       <c r="D260" s="99" t="s">
         <v>25</v>
@@ -59494,6 +59530,9 @@
       </c>
       <c r="Q260" s="100">
         <v>97</v>
+      </c>
+      <c r="R260" s="29" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -91073,7 +91112,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2021-05-25T11:48:33Z</value>
+      <value order="0">2021-05-25T15:58:12Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -91088,13 +91127,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA48848343</value>
+      <value order="0">vA48859668</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">78.106</value>
+      <value order="0">78.108</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">862</value>
+      <value order="0">864</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>